<commit_message>
Cleanup combined workbook formulas.
Do this to make them a little more defensible.
</commit_message>
<xml_diff>
--- a/0273NYP - New York Premier/NYHealth_Billing_Tracking.xlsx
+++ b/0273NYP - New York Premier/NYHealth_Billing_Tracking.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason.Altieri\repos\client-and-project-documentation\0273NYP - New York Premier\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shea.parkes\repos\client-and-project-documentation\0273NYP - New York Premier\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1395" yWindow="0" windowWidth="13680" windowHeight="13890" activeTab="2"/>
+    <workbookView xWindow="1400" yWindow="0" windowWidth="13680" windowHeight="13890"/>
   </bookViews>
   <sheets>
     <sheet name="Total" sheetId="9" r:id="rId1"/>
@@ -292,8 +292,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
-    <numFmt numFmtId="171" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -340,17 +340,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -358,22 +358,7 @@
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color theme="0" tint="-0.24994659260841701"/>
@@ -677,18 +662,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="10.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="1"/>
+    <col min="2" max="2" width="10.7265625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -700,48 +688,48 @@
       </c>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="6">
-        <f>SUM('Non-Collaborative'!B2:XFD2, Collaborative!B2:XFD2)</f>
+        <f>SUM('Non-Collaborative'!2:2, Collaborative!2:2)</f>
         <v>4495</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="6">
-        <f>SUM('Non-Collaborative'!B3:XFD3, Collaborative!B3:XFD3)</f>
+        <f>SUM('Non-Collaborative'!3:3, Collaborative!3:3)</f>
         <v>30601.04166666665</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="6">
-        <f>SUM('Non-Collaborative'!B4:XFD4, Collaborative!B4:XFD4)</f>
+        <f>SUM('Non-Collaborative'!4:4, Collaborative!4:4)</f>
         <v>30601.04166666665</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="6">
-        <f>SUM('Non-Collaborative'!B5:XFD5, Collaborative!B5:XFD5)</f>
+        <f>SUM('Non-Collaborative'!5:5, Collaborative!5:5)</f>
         <v>30601.04166666665</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="6">
-        <f>SUM('Non-Collaborative'!B6:XFD6, Collaborative!B6:XFD6)</f>
+        <f>SUM('Non-Collaborative'!6:6, Collaborative!6:6)</f>
         <v>30601.04166666665</v>
       </c>
       <c r="C6" s="7">
@@ -749,30 +737,30 @@
         <v>96298.124999999942</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="6">
-        <f>SUM('Non-Collaborative'!B7:XFD7, Collaborative!B7:XFD7)</f>
+        <f>SUM('Non-Collaborative'!7:7, Collaborative!7:7)</f>
         <v>30601.04166666665</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="6">
-        <f>SUM('Non-Collaborative'!B8:XFD8, Collaborative!B8:XFD8)</f>
+        <f>SUM('Non-Collaborative'!8:8, Collaborative!8:8)</f>
         <v>30601.04166666665</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="6">
-        <f>SUM('Non-Collaborative'!B9:XFD9, Collaborative!B9:XFD9)</f>
+        <f>SUM('Non-Collaborative'!9:9, Collaborative!9:9)</f>
         <v>30601.04166666665</v>
       </c>
       <c r="C9" s="7">
@@ -780,30 +768,30 @@
         <v>91803.124999999942</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="6">
-        <f>SUM('Non-Collaborative'!B10:XFD10, Collaborative!B10:XFD10)</f>
+        <f>SUM('Non-Collaborative'!10:10, Collaborative!10:10)</f>
         <v>30601.04166666665</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="6">
-        <f>SUM('Non-Collaborative'!B11:XFD11, Collaborative!B11:XFD11)</f>
+        <f>SUM('Non-Collaborative'!11:11, Collaborative!11:11)</f>
         <v>30601.04166666665</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="6">
-        <f>SUM('Non-Collaborative'!B12:XFD12, Collaborative!B12:XFD12)</f>
+        <f>SUM('Non-Collaborative'!12:12, Collaborative!12:12)</f>
         <v>30601.04166666665</v>
       </c>
       <c r="C12" s="7">
@@ -811,30 +799,30 @@
         <v>91803.124999999942</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="6">
-        <f>SUM('Non-Collaborative'!B13:XFD13, Collaborative!B13:XFD13)</f>
+        <f>SUM('Non-Collaborative'!13:13, Collaborative!13:13)</f>
         <v>30601.04166666665</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="6">
-        <f>SUM('Non-Collaborative'!B14:XFD14, Collaborative!B14:XFD14)</f>
+        <f>SUM('Non-Collaborative'!14:14, Collaborative!14:14)</f>
         <v>30601.04166666665</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="6">
-        <f>SUM('Non-Collaborative'!B15:XFD15, Collaborative!B15:XFD15)</f>
+        <f>SUM('Non-Collaborative'!15:15, Collaborative!15:15)</f>
         <v>30601.04166666665</v>
       </c>
       <c r="C15" s="7">
@@ -842,30 +830,30 @@
         <v>91803.124999999942</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="6">
-        <f>SUM('Non-Collaborative'!B16:XFD16, Collaborative!B16:XFD16)</f>
+        <f>SUM('Non-Collaborative'!16:16, Collaborative!16:16)</f>
         <v>30601.04166666665</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="6">
-        <f>SUM('Non-Collaborative'!B17:XFD17, Collaborative!B17:XFD17)</f>
+        <f>SUM('Non-Collaborative'!17:17, Collaborative!17:17)</f>
         <v>30601.04166666665</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="6">
-        <f>SUM('Non-Collaborative'!B18:XFD18, Collaborative!B18:XFD18)</f>
+        <f>SUM('Non-Collaborative'!18:18, Collaborative!18:18)</f>
         <v>30601.04166666665</v>
       </c>
       <c r="C18" s="7">
@@ -873,30 +861,30 @@
         <v>91803.124999999942</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="6">
-        <f>SUM('Non-Collaborative'!B19:XFD19, Collaborative!B19:XFD19)</f>
+        <f>SUM('Non-Collaborative'!19:19, Collaborative!19:19)</f>
         <v>30601.04166666665</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="6">
-        <f>SUM('Non-Collaborative'!B20:XFD20, Collaborative!B20:XFD20)</f>
+        <f>SUM('Non-Collaborative'!20:20, Collaborative!20:20)</f>
         <v>30601.04166666665</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="6">
-        <f>SUM('Non-Collaborative'!B21:XFD21, Collaborative!B21:XFD21)</f>
+        <f>SUM('Non-Collaborative'!21:21, Collaborative!21:21)</f>
         <v>30601.04166666665</v>
       </c>
       <c r="C21" s="7">
@@ -904,30 +892,30 @@
         <v>91803.124999999942</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="6">
-        <f>SUM('Non-Collaborative'!B22:XFD22, Collaborative!B22:XFD22)</f>
+        <f>SUM('Non-Collaborative'!22:22, Collaborative!22:22)</f>
         <v>30601.04166666665</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="6">
-        <f>SUM('Non-Collaborative'!B23:XFD23, Collaborative!B23:XFD23)</f>
+        <f>SUM('Non-Collaborative'!23:23, Collaborative!23:23)</f>
         <v>30601.04166666665</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="6">
-        <f>SUM('Non-Collaborative'!B24:XFD24, Collaborative!B24:XFD24)</f>
+        <f>SUM('Non-Collaborative'!24:24, Collaborative!24:24)</f>
         <v>30601.04166666665</v>
       </c>
       <c r="C24" s="7">
@@ -935,30 +923,30 @@
         <v>91803.124999999942</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B25" s="6">
-        <f>SUM('Non-Collaborative'!B25:XFD25, Collaborative!B25:XFD25)</f>
+        <f>SUM('Non-Collaborative'!25:25, Collaborative!25:25)</f>
         <v>30601.04166666665</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="6">
-        <f>SUM('Non-Collaborative'!B26:XFD26, Collaborative!B26:XFD26)</f>
+        <f>SUM('Non-Collaborative'!26:26, Collaborative!26:26)</f>
         <v>30601.04166666665</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="6">
-        <f>SUM('Non-Collaborative'!B27:XFD27, Collaborative!B27:XFD27)</f>
+        <f>SUM('Non-Collaborative'!27:27, Collaborative!27:27)</f>
         <v>30601.04166666665</v>
       </c>
       <c r="C27" s="7">
@@ -966,30 +954,30 @@
         <v>91803.124999999942</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="6">
-        <f>SUM('Non-Collaborative'!B28:XFD28, Collaborative!B28:XFD28)</f>
+        <f>SUM('Non-Collaborative'!28:28, Collaborative!28:28)</f>
         <v>30601.04166666665</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B29" s="6">
-        <f>SUM('Non-Collaborative'!B29:XFD29, Collaborative!B29:XFD29)</f>
+        <f>SUM('Non-Collaborative'!29:29, Collaborative!29:29)</f>
         <v>30601.04166666665</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B30" s="6">
-        <f>SUM('Non-Collaborative'!B30:XFD30, Collaborative!B30:XFD30)</f>
+        <f>SUM('Non-Collaborative'!30:30, Collaborative!30:30)</f>
         <v>30601.04166666665</v>
       </c>
       <c r="C30" s="7">
@@ -997,30 +985,30 @@
         <v>91803.124999999942</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B31" s="6">
-        <f>SUM('Non-Collaborative'!B31:XFD31, Collaborative!B31:XFD31)</f>
+        <f>SUM('Non-Collaborative'!31:31, Collaborative!31:31)</f>
         <v>30601.04166666665</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B32" s="6">
-        <f>SUM('Non-Collaborative'!B32:XFD32, Collaborative!B32:XFD32)</f>
+        <f>SUM('Non-Collaborative'!32:32, Collaborative!32:32)</f>
         <v>30601.04166666665</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B33" s="6">
-        <f>SUM('Non-Collaborative'!B33:XFD33, Collaborative!B33:XFD33)</f>
+        <f>SUM('Non-Collaborative'!33:33, Collaborative!33:33)</f>
         <v>28606.04166666665</v>
       </c>
       <c r="C33" s="7">
@@ -1028,30 +1016,30 @@
         <v>91803.124999999942</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B34" s="6">
-        <f>SUM('Non-Collaborative'!B34:XFD34, Collaborative!B34:XFD34)</f>
+        <f>SUM('Non-Collaborative'!34:34, Collaborative!34:34)</f>
         <v>28606.04166666665</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B35" s="6">
-        <f>SUM('Non-Collaborative'!B35:XFD35, Collaborative!B35:XFD35)</f>
+        <f>SUM('Non-Collaborative'!35:35, Collaborative!35:35)</f>
         <v>28606.04166666665</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B36" s="6">
-        <f>SUM('Non-Collaborative'!B36:XFD36, Collaborative!B36:XFD36)</f>
+        <f>SUM('Non-Collaborative'!36:36, Collaborative!36:36)</f>
         <v>28606.04166666665</v>
       </c>
       <c r="C36" s="7">
@@ -1059,30 +1047,30 @@
         <v>85818.124999999942</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B37" s="6">
-        <f>SUM('Non-Collaborative'!B37:XFD37, Collaborative!B37:XFD37)</f>
+        <f>SUM('Non-Collaborative'!37:37, Collaborative!37:37)</f>
         <v>28606.04166666665</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B38" s="6">
-        <f>SUM('Non-Collaborative'!B38:XFD38, Collaborative!B38:XFD38)</f>
+        <f>SUM('Non-Collaborative'!38:38, Collaborative!38:38)</f>
         <v>28606.04166666665</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B39" s="6">
-        <f>SUM('Non-Collaborative'!B39:XFD39, Collaborative!B39:XFD39)</f>
+        <f>SUM('Non-Collaborative'!39:39, Collaborative!39:39)</f>
         <v>0</v>
       </c>
       <c r="C39" s="7">
@@ -1090,25 +1078,25 @@
         <v>85818.124999999942</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B40" s="6">
-        <f>SUM('Non-Collaborative'!B40:XFD40, Collaborative!B40:XFD40)</f>
+        <f>SUM('Non-Collaborative'!40:40, Collaborative!40:40)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B41" s="6">
-        <f>SUM('Non-Collaborative'!B41:XFD41, Collaborative!B41:XFD41)</f>
+        <f>SUM('Non-Collaborative'!41:41, Collaborative!41:41)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C42" s="7">
         <f>SUM(B39:B41)</f>
         <v>0</v>
@@ -1123,13 +1111,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView topLeftCell="XEB1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1137,7 +1128,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1146,7 +1137,7 @@
         <v>4495</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1154,7 +1145,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1162,7 +1153,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1170,7 +1161,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1178,7 +1169,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1186,7 +1177,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1194,7 +1185,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1202,7 +1193,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1210,7 +1201,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1218,7 +1209,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1226,7 +1217,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1234,7 +1225,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1242,7 +1233,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1250,7 +1241,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1258,7 +1249,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1266,7 +1257,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1274,7 +1265,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1282,7 +1273,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1290,7 +1281,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1298,7 +1289,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1306,7 +1297,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1314,7 +1305,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1322,7 +1313,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1330,7 +1321,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1338,7 +1329,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1346,7 +1337,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1354,7 +1345,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -1362,7 +1353,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1370,7 +1361,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1378,7 +1369,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -1386,54 +1377,54 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>41</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B32">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1445,13 +1436,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="XEG25" sqref="XEG25"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1579,13 +1573,13 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1713,7 +1707,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1841,7 +1835,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1969,7 +1963,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -2097,7 +2091,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -2225,7 +2219,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -2353,7 +2347,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2481,7 +2475,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -2609,7 +2603,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -2737,7 +2731,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -2865,7 +2859,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -2993,7 +2987,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -3121,7 +3115,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -3249,7 +3243,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -3377,7 +3371,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -3505,7 +3499,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -3633,7 +3627,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -3761,7 +3755,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -3889,7 +3883,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -4017,7 +4011,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -4145,7 +4139,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -4273,7 +4267,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -4401,7 +4395,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -4529,7 +4523,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -4657,7 +4651,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -4785,7 +4779,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -4913,7 +4907,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -5041,7 +5035,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -5169,7 +5163,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -5297,7 +5291,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -5425,7 +5419,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="33" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -5553,7 +5547,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="34" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -5681,7 +5675,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="35" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -5809,7 +5803,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="36" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -5937,7 +5931,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="37" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -6065,7 +6059,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="38" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -6193,24 +6187,24 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="39" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>41</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update pricing model for 1111MCL
Do this because they upgraded to ACO Insight Enhanced.
</commit_message>
<xml_diff>
--- a/0273NYP - New York Premier/NYHealth_Billing_Tracking.xlsx
+++ b/0273NYP - New York Premier/NYHealth_Billing_Tracking.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shea.parkes\repos\client-and-project-documentation\0273NYP - New York Premier\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason.Altieri\repos\client-and-project-documentation\0273NYP - New York Premier\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="0" windowWidth="13680" windowHeight="13890"/>
+    <workbookView xWindow="1395" yWindow="0" windowWidth="13680" windowHeight="13890"/>
   </bookViews>
   <sheets>
     <sheet name="Total" sheetId="9" r:id="rId1"/>
@@ -358,7 +358,17 @@
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="0" tint="-0.24994659260841701"/>
@@ -669,14 +679,14 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="1"/>
-    <col min="2" max="2" width="10.7265625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="10.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -688,322 +698,322 @@
       </c>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="6">
         <f>SUM('Non-Collaborative'!2:2, Collaborative!2:2)</f>
-        <v>4495</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>4650</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="6">
         <f>SUM('Non-Collaborative'!3:3, Collaborative!3:3)</f>
-        <v>30601.04166666665</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>30756.041666666646</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="6">
         <f>SUM('Non-Collaborative'!4:4, Collaborative!4:4)</f>
-        <v>30601.04166666665</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+        <v>30756.041666666646</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="6">
         <f>SUM('Non-Collaborative'!5:5, Collaborative!5:5)</f>
-        <v>30601.04166666665</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+        <v>30756.041666666646</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="6">
         <f>SUM('Non-Collaborative'!6:6, Collaborative!6:6)</f>
-        <v>30601.04166666665</v>
+        <v>30756.041666666646</v>
       </c>
       <c r="C6" s="7">
         <f>SUM(B2:B5)</f>
-        <v>96298.124999999942</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+        <v>96918.124999999927</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="6">
         <f>SUM('Non-Collaborative'!7:7, Collaborative!7:7)</f>
-        <v>30601.04166666665</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+        <v>30756.041666666646</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="6">
         <f>SUM('Non-Collaborative'!8:8, Collaborative!8:8)</f>
-        <v>30601.04166666665</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+        <v>30756.041666666646</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="6">
         <f>SUM('Non-Collaborative'!9:9, Collaborative!9:9)</f>
-        <v>30601.04166666665</v>
+        <v>30756.041666666646</v>
       </c>
       <c r="C9" s="7">
         <f>SUM(B6:B8)</f>
-        <v>91803.124999999942</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+        <v>92268.124999999942</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="6">
         <f>SUM('Non-Collaborative'!10:10, Collaborative!10:10)</f>
-        <v>30601.04166666665</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+        <v>30756.041666666646</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="6">
         <f>SUM('Non-Collaborative'!11:11, Collaborative!11:11)</f>
-        <v>30601.04166666665</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+        <v>30756.041666666646</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="6">
         <f>SUM('Non-Collaborative'!12:12, Collaborative!12:12)</f>
-        <v>30601.04166666665</v>
+        <v>30756.041666666646</v>
       </c>
       <c r="C12" s="7">
         <f>SUM(B9:B11)</f>
-        <v>91803.124999999942</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+        <v>92268.124999999942</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="6">
         <f>SUM('Non-Collaborative'!13:13, Collaborative!13:13)</f>
-        <v>30601.04166666665</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+        <v>30756.041666666646</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="6">
         <f>SUM('Non-Collaborative'!14:14, Collaborative!14:14)</f>
-        <v>30601.04166666665</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+        <v>30756.041666666646</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="6">
         <f>SUM('Non-Collaborative'!15:15, Collaborative!15:15)</f>
-        <v>30601.04166666665</v>
+        <v>30756.041666666646</v>
       </c>
       <c r="C15" s="7">
         <f>SUM(B12:B14)</f>
-        <v>91803.124999999942</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+        <v>92268.124999999942</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="6">
         <f>SUM('Non-Collaborative'!16:16, Collaborative!16:16)</f>
-        <v>30601.04166666665</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+        <v>30756.041666666646</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="6">
         <f>SUM('Non-Collaborative'!17:17, Collaborative!17:17)</f>
-        <v>30601.04166666665</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+        <v>30756.041666666646</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="6">
         <f>SUM('Non-Collaborative'!18:18, Collaborative!18:18)</f>
-        <v>30601.04166666665</v>
+        <v>30756.041666666646</v>
       </c>
       <c r="C18" s="7">
         <f>SUM(B15:B17)</f>
-        <v>91803.124999999942</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+        <v>92268.124999999942</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="6">
         <f>SUM('Non-Collaborative'!19:19, Collaborative!19:19)</f>
-        <v>30601.04166666665</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+        <v>30756.041666666646</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="6">
         <f>SUM('Non-Collaborative'!20:20, Collaborative!20:20)</f>
-        <v>30601.04166666665</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+        <v>30756.041666666646</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="6">
         <f>SUM('Non-Collaborative'!21:21, Collaborative!21:21)</f>
-        <v>30601.04166666665</v>
+        <v>30756.041666666646</v>
       </c>
       <c r="C21" s="7">
         <f>SUM(B18:B20)</f>
-        <v>91803.124999999942</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+        <v>92268.124999999942</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="6">
         <f>SUM('Non-Collaborative'!22:22, Collaborative!22:22)</f>
-        <v>30601.04166666665</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+        <v>30756.041666666646</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="6">
         <f>SUM('Non-Collaborative'!23:23, Collaborative!23:23)</f>
-        <v>30601.04166666665</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+        <v>30756.041666666646</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="6">
         <f>SUM('Non-Collaborative'!24:24, Collaborative!24:24)</f>
-        <v>30601.04166666665</v>
+        <v>30756.041666666646</v>
       </c>
       <c r="C24" s="7">
         <f>SUM(B21:B23)</f>
-        <v>91803.124999999942</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+        <v>92268.124999999942</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B25" s="6">
         <f>SUM('Non-Collaborative'!25:25, Collaborative!25:25)</f>
-        <v>30601.04166666665</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+        <v>30756.041666666646</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="6">
         <f>SUM('Non-Collaborative'!26:26, Collaborative!26:26)</f>
-        <v>30601.04166666665</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+        <v>30756.041666666646</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="6">
         <f>SUM('Non-Collaborative'!27:27, Collaborative!27:27)</f>
-        <v>30601.04166666665</v>
+        <v>30756.041666666646</v>
       </c>
       <c r="C27" s="7">
         <f>SUM(B24:B26)</f>
-        <v>91803.124999999942</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+        <v>92268.124999999942</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="6">
         <f>SUM('Non-Collaborative'!28:28, Collaborative!28:28)</f>
-        <v>30601.04166666665</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+        <v>30756.041666666646</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B29" s="6">
         <f>SUM('Non-Collaborative'!29:29, Collaborative!29:29)</f>
-        <v>30601.04166666665</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+        <v>30756.041666666646</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B30" s="6">
         <f>SUM('Non-Collaborative'!30:30, Collaborative!30:30)</f>
-        <v>30601.04166666665</v>
+        <v>30756.041666666646</v>
       </c>
       <c r="C30" s="7">
         <f>SUM(B27:B29)</f>
-        <v>91803.124999999942</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+        <v>92268.124999999942</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B31" s="6">
         <f>SUM('Non-Collaborative'!31:31, Collaborative!31:31)</f>
-        <v>30601.04166666665</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+        <v>30756.041666666646</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B32" s="6">
         <f>SUM('Non-Collaborative'!32:32, Collaborative!32:32)</f>
-        <v>30601.04166666665</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+        <v>30756.041666666646</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
@@ -1013,10 +1023,10 @@
       </c>
       <c r="C33" s="7">
         <f>SUM(B30:B32)</f>
-        <v>91803.124999999942</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+        <v>92268.124999999942</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>34</v>
       </c>
@@ -1025,7 +1035,7 @@
         <v>28606.04166666665</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
@@ -1034,7 +1044,7 @@
         <v>28606.04166666665</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>36</v>
       </c>
@@ -1047,7 +1057,7 @@
         <v>85818.124999999942</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>37</v>
       </c>
@@ -1056,7 +1066,7 @@
         <v>28606.04166666665</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>38</v>
       </c>
@@ -1065,7 +1075,7 @@
         <v>28606.04166666665</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>39</v>
       </c>
@@ -1078,7 +1088,7 @@
         <v>85818.124999999942</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>40</v>
       </c>
@@ -1087,7 +1097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>41</v>
       </c>
@@ -1096,7 +1106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C42" s="7">
         <f>SUM(B39:B41)</f>
         <v>0</v>
@@ -1115,12 +1125,12 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1128,303 +1138,303 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3">
-        <f>1995+2500</f>
-        <v>4495</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <f>2500+2150</f>
+        <v>4650</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="3">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="3">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="3">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="3">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="3">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="3">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="3">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="3">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="3">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="3">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="3">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="3">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="3">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="3">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="3">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="3">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="3">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="3">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="3">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="3">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
       <c r="B25" s="3">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="3">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="3">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="3">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
       <c r="B29" s="3">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
       <c r="B30" s="3">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
       <c r="B31" s="3">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
       <c r="B32" s="3">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B32">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1443,9 +1453,9 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1573,13 +1583,13 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1707,7 +1717,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1835,7 +1845,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1963,7 +1973,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -2091,7 +2101,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -2219,7 +2229,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -2347,7 +2357,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2475,7 +2485,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -2603,7 +2613,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -2731,7 +2741,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -2859,7 +2869,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -2987,7 +2997,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -3115,7 +3125,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -3243,7 +3253,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -3371,7 +3381,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -3499,7 +3509,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -3627,7 +3637,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -3755,7 +3765,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -3883,7 +3893,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -4011,7 +4021,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -4139,7 +4149,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -4267,7 +4277,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -4395,7 +4405,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -4523,7 +4533,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="26" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -4651,7 +4661,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -4779,7 +4789,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -4907,7 +4917,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="29" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -5035,7 +5045,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="30" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -5163,7 +5173,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="31" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -5291,7 +5301,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="32" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -5419,7 +5429,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="33" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -5547,7 +5557,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="34" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -5675,7 +5685,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="35" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -5803,7 +5813,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="36" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -5931,7 +5941,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="37" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -6059,7 +6069,7 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="38" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -6187,34 +6197,34 @@
         <v>697.70833333333337</v>
       </c>
     </row>
-    <row r="39" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B38">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:AP38">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update billing tracking spreadsheet
Do this to include the fact we are now billing for the MI royalties
</commit_message>
<xml_diff>
--- a/0273NYP - New York Premier/NYHealth_Billing_Tracking.xlsx
+++ b/0273NYP - New York Premier/NYHealth_Billing_Tracking.xlsx
@@ -358,17 +358,7 @@
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color theme="0" tint="-0.24994659260841701"/>
@@ -676,7 +666,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,7 +694,7 @@
       </c>
       <c r="B2" s="6">
         <f>SUM('Non-Collaborative'!2:2, Collaborative!2:2)</f>
-        <v>4650</v>
+        <v>5250</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -713,7 +703,7 @@
       </c>
       <c r="B3" s="6">
         <f>SUM('Non-Collaborative'!3:3, Collaborative!3:3)</f>
-        <v>30756.041666666646</v>
+        <v>31356.041666666646</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -722,7 +712,7 @@
       </c>
       <c r="B4" s="6">
         <f>SUM('Non-Collaborative'!4:4, Collaborative!4:4)</f>
-        <v>30756.041666666646</v>
+        <v>31356.041666666646</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -731,7 +721,7 @@
       </c>
       <c r="B5" s="6">
         <f>SUM('Non-Collaborative'!5:5, Collaborative!5:5)</f>
-        <v>30756.041666666646</v>
+        <v>31356.041666666646</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -740,11 +730,11 @@
       </c>
       <c r="B6" s="6">
         <f>SUM('Non-Collaborative'!6:6, Collaborative!6:6)</f>
-        <v>30756.041666666646</v>
+        <v>31356.041666666646</v>
       </c>
       <c r="C6" s="7">
         <f>SUM(B2:B5)</f>
-        <v>96918.124999999927</v>
+        <v>99318.124999999927</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -753,7 +743,7 @@
       </c>
       <c r="B7" s="6">
         <f>SUM('Non-Collaborative'!7:7, Collaborative!7:7)</f>
-        <v>30756.041666666646</v>
+        <v>31356.041666666646</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -762,7 +752,7 @@
       </c>
       <c r="B8" s="6">
         <f>SUM('Non-Collaborative'!8:8, Collaborative!8:8)</f>
-        <v>30756.041666666646</v>
+        <v>31356.041666666646</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -771,11 +761,11 @@
       </c>
       <c r="B9" s="6">
         <f>SUM('Non-Collaborative'!9:9, Collaborative!9:9)</f>
-        <v>30756.041666666646</v>
+        <v>31356.041666666646</v>
       </c>
       <c r="C9" s="7">
         <f>SUM(B6:B8)</f>
-        <v>92268.124999999942</v>
+        <v>94068.124999999942</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -784,7 +774,7 @@
       </c>
       <c r="B10" s="6">
         <f>SUM('Non-Collaborative'!10:10, Collaborative!10:10)</f>
-        <v>30756.041666666646</v>
+        <v>31356.041666666646</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -793,7 +783,7 @@
       </c>
       <c r="B11" s="6">
         <f>SUM('Non-Collaborative'!11:11, Collaborative!11:11)</f>
-        <v>30756.041666666646</v>
+        <v>31356.041666666646</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -802,11 +792,11 @@
       </c>
       <c r="B12" s="6">
         <f>SUM('Non-Collaborative'!12:12, Collaborative!12:12)</f>
-        <v>30756.041666666646</v>
+        <v>31356.041666666646</v>
       </c>
       <c r="C12" s="7">
         <f>SUM(B9:B11)</f>
-        <v>92268.124999999942</v>
+        <v>94068.124999999942</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -815,7 +805,7 @@
       </c>
       <c r="B13" s="6">
         <f>SUM('Non-Collaborative'!13:13, Collaborative!13:13)</f>
-        <v>30756.041666666646</v>
+        <v>31356.041666666646</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -824,7 +814,7 @@
       </c>
       <c r="B14" s="6">
         <f>SUM('Non-Collaborative'!14:14, Collaborative!14:14)</f>
-        <v>30756.041666666646</v>
+        <v>31356.041666666646</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -833,11 +823,11 @@
       </c>
       <c r="B15" s="6">
         <f>SUM('Non-Collaborative'!15:15, Collaborative!15:15)</f>
-        <v>30756.041666666646</v>
+        <v>31356.041666666646</v>
       </c>
       <c r="C15" s="7">
         <f>SUM(B12:B14)</f>
-        <v>92268.124999999942</v>
+        <v>94068.124999999942</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -846,7 +836,7 @@
       </c>
       <c r="B16" s="6">
         <f>SUM('Non-Collaborative'!16:16, Collaborative!16:16)</f>
-        <v>30756.041666666646</v>
+        <v>31356.041666666646</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -855,7 +845,7 @@
       </c>
       <c r="B17" s="6">
         <f>SUM('Non-Collaborative'!17:17, Collaborative!17:17)</f>
-        <v>30756.041666666646</v>
+        <v>31356.041666666646</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -864,11 +854,11 @@
       </c>
       <c r="B18" s="6">
         <f>SUM('Non-Collaborative'!18:18, Collaborative!18:18)</f>
-        <v>30756.041666666646</v>
+        <v>31356.041666666646</v>
       </c>
       <c r="C18" s="7">
         <f>SUM(B15:B17)</f>
-        <v>92268.124999999942</v>
+        <v>94068.124999999942</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -877,7 +867,7 @@
       </c>
       <c r="B19" s="6">
         <f>SUM('Non-Collaborative'!19:19, Collaborative!19:19)</f>
-        <v>30756.041666666646</v>
+        <v>31356.041666666646</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -886,7 +876,7 @@
       </c>
       <c r="B20" s="6">
         <f>SUM('Non-Collaborative'!20:20, Collaborative!20:20)</f>
-        <v>30756.041666666646</v>
+        <v>31356.041666666646</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -895,11 +885,11 @@
       </c>
       <c r="B21" s="6">
         <f>SUM('Non-Collaborative'!21:21, Collaborative!21:21)</f>
-        <v>30756.041666666646</v>
+        <v>31356.041666666646</v>
       </c>
       <c r="C21" s="7">
         <f>SUM(B18:B20)</f>
-        <v>92268.124999999942</v>
+        <v>94068.124999999942</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -908,7 +898,7 @@
       </c>
       <c r="B22" s="6">
         <f>SUM('Non-Collaborative'!22:22, Collaborative!22:22)</f>
-        <v>30756.041666666646</v>
+        <v>31356.041666666646</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -917,7 +907,7 @@
       </c>
       <c r="B23" s="6">
         <f>SUM('Non-Collaborative'!23:23, Collaborative!23:23)</f>
-        <v>30756.041666666646</v>
+        <v>31356.041666666646</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -926,11 +916,11 @@
       </c>
       <c r="B24" s="6">
         <f>SUM('Non-Collaborative'!24:24, Collaborative!24:24)</f>
-        <v>30756.041666666646</v>
+        <v>31356.041666666646</v>
       </c>
       <c r="C24" s="7">
         <f>SUM(B21:B23)</f>
-        <v>92268.124999999942</v>
+        <v>94068.124999999942</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -939,7 +929,7 @@
       </c>
       <c r="B25" s="6">
         <f>SUM('Non-Collaborative'!25:25, Collaborative!25:25)</f>
-        <v>30756.041666666646</v>
+        <v>31356.041666666646</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -948,7 +938,7 @@
       </c>
       <c r="B26" s="6">
         <f>SUM('Non-Collaborative'!26:26, Collaborative!26:26)</f>
-        <v>30756.041666666646</v>
+        <v>31356.041666666646</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -957,11 +947,11 @@
       </c>
       <c r="B27" s="6">
         <f>SUM('Non-Collaborative'!27:27, Collaborative!27:27)</f>
-        <v>30756.041666666646</v>
+        <v>31356.041666666646</v>
       </c>
       <c r="C27" s="7">
         <f>SUM(B24:B26)</f>
-        <v>92268.124999999942</v>
+        <v>94068.124999999942</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -970,7 +960,7 @@
       </c>
       <c r="B28" s="6">
         <f>SUM('Non-Collaborative'!28:28, Collaborative!28:28)</f>
-        <v>30756.041666666646</v>
+        <v>31356.041666666646</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -979,7 +969,7 @@
       </c>
       <c r="B29" s="6">
         <f>SUM('Non-Collaborative'!29:29, Collaborative!29:29)</f>
-        <v>30756.041666666646</v>
+        <v>31356.041666666646</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -988,11 +978,11 @@
       </c>
       <c r="B30" s="6">
         <f>SUM('Non-Collaborative'!30:30, Collaborative!30:30)</f>
-        <v>30756.041666666646</v>
+        <v>31356.041666666646</v>
       </c>
       <c r="C30" s="7">
         <f>SUM(B27:B29)</f>
-        <v>92268.124999999942</v>
+        <v>94068.124999999942</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1001,7 +991,7 @@
       </c>
       <c r="B31" s="6">
         <f>SUM('Non-Collaborative'!31:31, Collaborative!31:31)</f>
-        <v>30756.041666666646</v>
+        <v>31356.041666666646</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1010,7 +1000,7 @@
       </c>
       <c r="B32" s="6">
         <f>SUM('Non-Collaborative'!32:32, Collaborative!32:32)</f>
-        <v>30756.041666666646</v>
+        <v>31356.041666666646</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1023,7 +1013,7 @@
       </c>
       <c r="C33" s="7">
         <f>SUM(B30:B32)</f>
-        <v>92268.124999999942</v>
+        <v>94068.124999999942</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1125,7 +1115,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1143,8 +1133,8 @@
         <v>2</v>
       </c>
       <c r="B2" s="3">
-        <f>2500+2150</f>
-        <v>4650</v>
+        <f>2500+2270+480</f>
+        <v>5250</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1152,7 +1142,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3">
-        <v>2150</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1160,7 +1150,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="3">
-        <v>2150</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1168,7 +1158,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="3">
-        <v>2150</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1176,7 +1166,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="3">
-        <v>2150</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1184,7 +1174,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="3">
-        <v>2150</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1192,7 +1182,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="3">
-        <v>2150</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1200,7 +1190,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="3">
-        <v>2150</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1208,7 +1198,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="3">
-        <v>2150</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1216,7 +1206,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="3">
-        <v>2150</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1224,7 +1214,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="3">
-        <v>2150</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1232,7 +1222,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="3">
-        <v>2150</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1240,7 +1230,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="3">
-        <v>2150</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1248,7 +1238,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="3">
-        <v>2150</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1256,7 +1246,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="3">
-        <v>2150</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1264,7 +1254,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="3">
-        <v>2150</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1272,7 +1262,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="3">
-        <v>2150</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1280,7 +1270,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="3">
-        <v>2150</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1288,7 +1278,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="3">
-        <v>2150</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1296,7 +1286,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="3">
-        <v>2150</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1304,7 +1294,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="3">
-        <v>2150</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1312,7 +1302,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="3">
-        <v>2150</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1320,7 +1310,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="3">
-        <v>2150</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1328,7 +1318,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="3">
-        <v>2150</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1336,7 +1326,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="3">
-        <v>2150</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1344,7 +1334,7 @@
         <v>27</v>
       </c>
       <c r="B27" s="3">
-        <v>2150</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -1352,7 +1342,7 @@
         <v>28</v>
       </c>
       <c r="B28" s="3">
-        <v>2150</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1360,7 +1350,7 @@
         <v>29</v>
       </c>
       <c r="B29" s="3">
-        <v>2150</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -1368,7 +1358,7 @@
         <v>30</v>
       </c>
       <c r="B30" s="3">
-        <v>2150</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1376,7 +1366,7 @@
         <v>31</v>
       </c>
       <c r="B31" s="3">
-        <v>2150</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1384,7 +1374,7 @@
         <v>32</v>
       </c>
       <c r="B32" s="3">
-        <v>2150</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
@@ -1434,7 +1424,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B32">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1450,7 +1440,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6214,17 +6204,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B38">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:AP38">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Split out MI royalties in tracking sheet
Do this for easier billing
</commit_message>
<xml_diff>
--- a/0273NYP - New York Premier/NYHealth_Billing_Tracking.xlsx
+++ b/0273NYP - New York Premier/NYHealth_Billing_Tracking.xlsx
@@ -15,8 +15,10 @@
     <sheet name="Total" sheetId="9" r:id="rId1"/>
     <sheet name="Non-Collaborative" sheetId="10" r:id="rId2"/>
     <sheet name="Collaborative" sheetId="11" r:id="rId3"/>
+    <sheet name="MI_Royalties" sheetId="12" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="ACOInsight1" localSheetId="3">#REF!</definedName>
     <definedName name="ACOInsight1">#REF!</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="87">
   <si>
     <t>Month</t>
   </si>
@@ -284,6 +286,12 @@
   </si>
   <si>
     <t>All Clients Monthly</t>
+  </si>
+  <si>
+    <t>MI Royalties</t>
+  </si>
+  <si>
+    <t>MI Royalties Quarterly</t>
   </si>
 </sst>
 </file>
@@ -332,7 +340,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -341,9 +349,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -358,7 +363,17 @@
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="0" tint="-0.24994659260841701"/>
@@ -660,13 +675,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomRight" activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,430 +689,645 @@
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="10.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="10.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <f>SUM('Non-Collaborative'!2:2, Collaborative!2:2)</f>
-        <v>5250</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4770</v>
+      </c>
+      <c r="D2">
+        <f>SUM(MI_Royalties!B2:XFD2)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <f>SUM('Non-Collaborative'!3:3, Collaborative!3:3)</f>
-        <v>31356.041666666646</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>30876.041666666646</v>
+      </c>
+      <c r="D3">
+        <f>SUM(MI_Royalties!B3:XFD3)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <f>SUM('Non-Collaborative'!4:4, Collaborative!4:4)</f>
-        <v>31356.041666666646</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>30876.041666666646</v>
+      </c>
+      <c r="D4">
+        <f>SUM(MI_Royalties!B4:XFD4)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <f>SUM('Non-Collaborative'!5:5, Collaborative!5:5)</f>
-        <v>31356.041666666646</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>30876.041666666646</v>
+      </c>
+      <c r="D5">
+        <f>SUM(MI_Royalties!B5:XFD5)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <f>SUM('Non-Collaborative'!6:6, Collaborative!6:6)</f>
-        <v>31356.041666666646</v>
-      </c>
-      <c r="C6" s="7">
+        <v>30876.041666666646</v>
+      </c>
+      <c r="C6" s="6">
         <f>SUM(B2:B5)</f>
-        <v>99318.124999999927</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>97398.124999999927</v>
+      </c>
+      <c r="D6">
+        <f>SUM(MI_Royalties!B6:XFD6)</f>
+        <v>480</v>
+      </c>
+      <c r="E6" s="6">
+        <f>SUM(D2:D5)</f>
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <f>SUM('Non-Collaborative'!7:7, Collaborative!7:7)</f>
-        <v>31356.041666666646</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>30876.041666666646</v>
+      </c>
+      <c r="D7">
+        <f>SUM(MI_Royalties!B7:XFD7)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <f>SUM('Non-Collaborative'!8:8, Collaborative!8:8)</f>
-        <v>31356.041666666646</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>30876.041666666646</v>
+      </c>
+      <c r="D8">
+        <f>SUM(MI_Royalties!B8:XFD8)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <f>SUM('Non-Collaborative'!9:9, Collaborative!9:9)</f>
-        <v>31356.041666666646</v>
-      </c>
-      <c r="C9" s="7">
+        <v>30876.041666666646</v>
+      </c>
+      <c r="C9" s="6">
         <f>SUM(B6:B8)</f>
-        <v>94068.124999999942</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>92628.124999999942</v>
+      </c>
+      <c r="D9">
+        <f>SUM(MI_Royalties!B9:XFD9)</f>
+        <v>480</v>
+      </c>
+      <c r="E9" s="6">
+        <f>SUM(D5:D8)</f>
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <f>SUM('Non-Collaborative'!10:10, Collaborative!10:10)</f>
-        <v>31356.041666666646</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>30876.041666666646</v>
+      </c>
+      <c r="D10">
+        <f>SUM(MI_Royalties!B10:XFD10)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <f>SUM('Non-Collaborative'!11:11, Collaborative!11:11)</f>
-        <v>31356.041666666646</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>30876.041666666646</v>
+      </c>
+      <c r="D11">
+        <f>SUM(MI_Royalties!B11:XFD11)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="5">
         <f>SUM('Non-Collaborative'!12:12, Collaborative!12:12)</f>
-        <v>31356.041666666646</v>
-      </c>
-      <c r="C12" s="7">
+        <v>30876.041666666646</v>
+      </c>
+      <c r="C12" s="6">
         <f>SUM(B9:B11)</f>
-        <v>94068.124999999942</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>92628.124999999942</v>
+      </c>
+      <c r="D12">
+        <f>SUM(MI_Royalties!B12:XFD12)</f>
+        <v>480</v>
+      </c>
+      <c r="E12" s="6">
+        <f>SUM(D8:D11)</f>
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <f>SUM('Non-Collaborative'!13:13, Collaborative!13:13)</f>
-        <v>31356.041666666646</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>30876.041666666646</v>
+      </c>
+      <c r="D13">
+        <f>SUM(MI_Royalties!B13:XFD13)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="5">
         <f>SUM('Non-Collaborative'!14:14, Collaborative!14:14)</f>
-        <v>31356.041666666646</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>30876.041666666646</v>
+      </c>
+      <c r="D14">
+        <f>SUM(MI_Royalties!B14:XFD14)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="5">
         <f>SUM('Non-Collaborative'!15:15, Collaborative!15:15)</f>
-        <v>31356.041666666646</v>
-      </c>
-      <c r="C15" s="7">
+        <v>30876.041666666646</v>
+      </c>
+      <c r="C15" s="6">
         <f>SUM(B12:B14)</f>
-        <v>94068.124999999942</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>92628.124999999942</v>
+      </c>
+      <c r="D15">
+        <f>SUM(MI_Royalties!B15:XFD15)</f>
+        <v>480</v>
+      </c>
+      <c r="E15" s="6">
+        <f>SUM(D11:D14)</f>
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="5">
         <f>SUM('Non-Collaborative'!16:16, Collaborative!16:16)</f>
-        <v>31356.041666666646</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30876.041666666646</v>
+      </c>
+      <c r="D16">
+        <f>SUM(MI_Royalties!B16:XFD16)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="5">
         <f>SUM('Non-Collaborative'!17:17, Collaborative!17:17)</f>
-        <v>31356.041666666646</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30876.041666666646</v>
+      </c>
+      <c r="D17">
+        <f>SUM(MI_Royalties!B17:XFD17)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="5">
         <f>SUM('Non-Collaborative'!18:18, Collaborative!18:18)</f>
-        <v>31356.041666666646</v>
-      </c>
-      <c r="C18" s="7">
+        <v>30876.041666666646</v>
+      </c>
+      <c r="C18" s="6">
         <f>SUM(B15:B17)</f>
-        <v>94068.124999999942</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92628.124999999942</v>
+      </c>
+      <c r="D18">
+        <f>SUM(MI_Royalties!B18:XFD18)</f>
+        <v>480</v>
+      </c>
+      <c r="E18" s="6">
+        <f>SUM(D14:D17)</f>
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="5">
         <f>SUM('Non-Collaborative'!19:19, Collaborative!19:19)</f>
-        <v>31356.041666666646</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30876.041666666646</v>
+      </c>
+      <c r="D19">
+        <f>SUM(MI_Royalties!B19:XFD19)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="5">
         <f>SUM('Non-Collaborative'!20:20, Collaborative!20:20)</f>
-        <v>31356.041666666646</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30876.041666666646</v>
+      </c>
+      <c r="D20">
+        <f>SUM(MI_Royalties!B20:XFD20)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="5">
         <f>SUM('Non-Collaborative'!21:21, Collaborative!21:21)</f>
-        <v>31356.041666666646</v>
-      </c>
-      <c r="C21" s="7">
+        <v>30876.041666666646</v>
+      </c>
+      <c r="C21" s="6">
         <f>SUM(B18:B20)</f>
-        <v>94068.124999999942</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92628.124999999942</v>
+      </c>
+      <c r="D21">
+        <f>SUM(MI_Royalties!B21:XFD21)</f>
+        <v>480</v>
+      </c>
+      <c r="E21" s="6">
+        <f>SUM(D17:D20)</f>
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="5">
         <f>SUM('Non-Collaborative'!22:22, Collaborative!22:22)</f>
-        <v>31356.041666666646</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30876.041666666646</v>
+      </c>
+      <c r="D22">
+        <f>SUM(MI_Royalties!B22:XFD22)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="5">
         <f>SUM('Non-Collaborative'!23:23, Collaborative!23:23)</f>
-        <v>31356.041666666646</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30876.041666666646</v>
+      </c>
+      <c r="D23">
+        <f>SUM(MI_Royalties!B23:XFD23)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="5">
         <f>SUM('Non-Collaborative'!24:24, Collaborative!24:24)</f>
-        <v>31356.041666666646</v>
-      </c>
-      <c r="C24" s="7">
+        <v>30876.041666666646</v>
+      </c>
+      <c r="C24" s="6">
         <f>SUM(B21:B23)</f>
-        <v>94068.124999999942</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92628.124999999942</v>
+      </c>
+      <c r="D24">
+        <f>SUM(MI_Royalties!B24:XFD24)</f>
+        <v>480</v>
+      </c>
+      <c r="E24" s="6">
+        <f>SUM(D20:D23)</f>
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="5">
         <f>SUM('Non-Collaborative'!25:25, Collaborative!25:25)</f>
-        <v>31356.041666666646</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30876.041666666646</v>
+      </c>
+      <c r="D25">
+        <f>SUM(MI_Royalties!B25:XFD25)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="5">
         <f>SUM('Non-Collaborative'!26:26, Collaborative!26:26)</f>
-        <v>31356.041666666646</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30876.041666666646</v>
+      </c>
+      <c r="D26">
+        <f>SUM(MI_Royalties!B26:XFD26)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="5">
         <f>SUM('Non-Collaborative'!27:27, Collaborative!27:27)</f>
-        <v>31356.041666666646</v>
-      </c>
-      <c r="C27" s="7">
+        <v>30876.041666666646</v>
+      </c>
+      <c r="C27" s="6">
         <f>SUM(B24:B26)</f>
-        <v>94068.124999999942</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92628.124999999942</v>
+      </c>
+      <c r="D27">
+        <f>SUM(MI_Royalties!B27:XFD27)</f>
+        <v>480</v>
+      </c>
+      <c r="E27" s="6">
+        <f>SUM(D23:D26)</f>
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="5">
         <f>SUM('Non-Collaborative'!28:28, Collaborative!28:28)</f>
-        <v>31356.041666666646</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30876.041666666646</v>
+      </c>
+      <c r="D28">
+        <f>SUM(MI_Royalties!B28:XFD28)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="5">
         <f>SUM('Non-Collaborative'!29:29, Collaborative!29:29)</f>
-        <v>31356.041666666646</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30876.041666666646</v>
+      </c>
+      <c r="D29">
+        <f>SUM(MI_Royalties!B29:XFD29)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30" s="5">
         <f>SUM('Non-Collaborative'!30:30, Collaborative!30:30)</f>
-        <v>31356.041666666646</v>
-      </c>
-      <c r="C30" s="7">
+        <v>30876.041666666646</v>
+      </c>
+      <c r="C30" s="6">
         <f>SUM(B27:B29)</f>
-        <v>94068.124999999942</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92628.124999999942</v>
+      </c>
+      <c r="D30">
+        <f>SUM(MI_Royalties!B30:XFD30)</f>
+        <v>480</v>
+      </c>
+      <c r="E30" s="6">
+        <f>SUM(D26:D29)</f>
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="5">
         <f>SUM('Non-Collaborative'!31:31, Collaborative!31:31)</f>
-        <v>31356.041666666646</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30876.041666666646</v>
+      </c>
+      <c r="D31">
+        <f>SUM(MI_Royalties!B31:XFD31)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B32" s="5">
         <f>SUM('Non-Collaborative'!32:32, Collaborative!32:32)</f>
-        <v>31356.041666666646</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30876.041666666646</v>
+      </c>
+      <c r="D32">
+        <f>SUM(MI_Royalties!B32:XFD32)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="6">
+      <c r="B33" s="5">
         <f>SUM('Non-Collaborative'!33:33, Collaborative!33:33)</f>
         <v>28606.04166666665</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C33" s="6">
         <f>SUM(B30:B32)</f>
-        <v>94068.124999999942</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92628.124999999942</v>
+      </c>
+      <c r="D33">
+        <f>SUM(MI_Royalties!B33:XFD33)</f>
+        <v>0</v>
+      </c>
+      <c r="E33" s="6">
+        <f>SUM(D29:D32)</f>
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="6">
+      <c r="B34" s="5">
         <f>SUM('Non-Collaborative'!34:34, Collaborative!34:34)</f>
         <v>28606.04166666665</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <f>SUM(MI_Royalties!B34:XFD34)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="6">
+      <c r="B35" s="5">
         <f>SUM('Non-Collaborative'!35:35, Collaborative!35:35)</f>
         <v>28606.04166666665</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <f>SUM(MI_Royalties!B35:XFD35)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B36" s="5">
         <f>SUM('Non-Collaborative'!36:36, Collaborative!36:36)</f>
         <v>28606.04166666665</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C36" s="6">
         <f>SUM(B33:B35)</f>
         <v>85818.124999999942</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <f>SUM(MI_Royalties!B36:XFD36)</f>
+        <v>0</v>
+      </c>
+      <c r="E36" s="6">
+        <f>SUM(D32:D35)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="6">
+      <c r="B37" s="5">
         <f>SUM('Non-Collaborative'!37:37, Collaborative!37:37)</f>
         <v>28606.04166666665</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <f>SUM(MI_Royalties!B37:XFD37)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="6">
+      <c r="B38" s="5">
         <f>SUM('Non-Collaborative'!38:38, Collaborative!38:38)</f>
         <v>28606.04166666665</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <f>SUM(MI_Royalties!B38:XFD38)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="6">
+      <c r="B39" s="5">
         <f>SUM('Non-Collaborative'!39:39, Collaborative!39:39)</f>
         <v>0</v>
       </c>
-      <c r="C39" s="7">
+      <c r="C39" s="6">
         <f>SUM(B36:B38)</f>
         <v>85818.124999999942</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <f>SUM(MI_Royalties!B39:XFD39)</f>
+        <v>0</v>
+      </c>
+      <c r="E39" s="6">
+        <f>SUM(D35:D38)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="6">
+      <c r="B40" s="5">
         <f>SUM('Non-Collaborative'!40:40, Collaborative!40:40)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <f>SUM(MI_Royalties!B40:XFD40)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="6">
+      <c r="B41" s="5">
         <f>SUM('Non-Collaborative'!41:41, Collaborative!41:41)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C42" s="7">
+      <c r="D41">
+        <f>SUM(MI_Royalties!B41:XFD41)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C42" s="6">
         <f>SUM(B39:B41)</f>
         <v>0</v>
       </c>
@@ -1115,7 +1345,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1133,8 +1363,8 @@
         <v>2</v>
       </c>
       <c r="B2" s="3">
-        <f>2500+2270+480</f>
-        <v>5250</v>
+        <f>2500+2270</f>
+        <v>4770</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1142,7 +1372,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3">
-        <v>2750</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1150,7 +1380,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="3">
-        <v>2750</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1158,7 +1388,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="3">
-        <v>2750</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1166,7 +1396,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="3">
-        <v>2750</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1174,7 +1404,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="3">
-        <v>2750</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1182,7 +1412,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="3">
-        <v>2750</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1190,7 +1420,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="3">
-        <v>2750</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1198,7 +1428,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="3">
-        <v>2750</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1206,7 +1436,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="3">
-        <v>2750</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1214,7 +1444,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="3">
-        <v>2750</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1222,7 +1452,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="3">
-        <v>2750</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1230,7 +1460,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="3">
-        <v>2750</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1238,7 +1468,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="3">
-        <v>2750</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1246,7 +1476,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="3">
-        <v>2750</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1254,7 +1484,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="3">
-        <v>2750</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1262,7 +1492,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="3">
-        <v>2750</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1270,7 +1500,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="3">
-        <v>2750</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1278,7 +1508,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="3">
-        <v>2750</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1286,7 +1516,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="3">
-        <v>2750</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1294,7 +1524,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="3">
-        <v>2750</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1302,7 +1532,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="3">
-        <v>2750</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1310,7 +1540,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="3">
-        <v>2750</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1318,7 +1548,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="3">
-        <v>2750</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1326,7 +1556,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="3">
-        <v>2750</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1334,7 +1564,7 @@
         <v>27</v>
       </c>
       <c r="B27" s="3">
-        <v>2750</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -1342,7 +1572,7 @@
         <v>28</v>
       </c>
       <c r="B28" s="3">
-        <v>2750</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1350,7 +1580,7 @@
         <v>29</v>
       </c>
       <c r="B29" s="3">
-        <v>2750</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -1358,7 +1588,7 @@
         <v>30</v>
       </c>
       <c r="B30" s="3">
-        <v>2750</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1366,7 +1596,7 @@
         <v>31</v>
       </c>
       <c r="B31" s="3">
-        <v>2750</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1374,7 +1604,7 @@
         <v>32</v>
       </c>
       <c r="B32" s="3">
-        <v>2750</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
@@ -1424,7 +1654,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B32">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6204,17 +6434,341 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B38">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:AP38">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="XEC2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="I23" sqref="I23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:B32">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>